<commit_message>
Validation case now includes graphs for K and P
</commit_message>
<xml_diff>
--- a/working_model/multiple runs/results/case_r.xlsx
+++ b/working_model/multiple runs/results/case_r.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\G drive ucsb\Quota Basket GP Folders\Model\Model in R\winterversion\quotabasket_model\working_model\multiple runs\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FFB13785-88D7-46D1-9AA9-8E4E7EB8F000}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DEE6D0F-D9AE-4819-A88B-D511C8D2E6BD}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="12036" yWindow="3048" windowWidth="9816" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -60,13 +60,13 @@
     <t>max</t>
   </si>
   <si>
-    <t>All same</t>
+    <t>All_same</t>
   </si>
   <si>
-    <t>Very different</t>
+    <t>Very_different</t>
   </si>
   <si>
-    <t>Somewhat different</t>
+    <t>Somewhat_different</t>
   </si>
 </sst>
 </file>
@@ -412,7 +412,7 @@
   <dimension ref="A1:K21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M6" sqref="M6"/>
+      <selection activeCell="I1" sqref="I1:K1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -452,13 +452,13 @@
       <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="I1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="J1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="K1" t="s">
         <v>10</v>
       </c>
     </row>

</xml_diff>